<commit_message>
Olink to Cimac_ID linkage (#194)
* Updated prismify to additionally return npx parsed list

* Modified prismify to return olink metadata_files

* move parse_npx to prism and update parse_npx

* Added attribute to LocalFileUploadEntry

* Added property 'metadata files'

* get field 'extra_metadata' from assay_template

* npx patch function

* EXTRA_METADATA_PARSERS

* parse_npx rejects filepaths

* create merge_artifact_extra_metadata

* create update_artifact

* update test for olink

* update extra_metadata test

* bump version to 0.6.2

* aliquot->cimac_id
</commit_message>
<xml_diff>
--- a/tests/data/olink/olink_assay_1_NPX.xlsx
+++ b/tests/data/olink/olink_assay_1_NPX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/Projects/CIDC/assay/olink/cidc_example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/tests/data/olink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36ADFA85-4E63-064D-805E-EBA75DC64EE7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9DE92E-168E-0145-A7A5-894EE03ECBDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63340" yWindow="5820" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NPX Data" sheetId="1" r:id="rId1"/>
@@ -880,31 +880,31 @@
     <t>OID00562</t>
   </si>
   <si>
-    <t>HD_59</t>
-  </si>
-  <si>
     <t>HIMC_CART_DEP_CHEAR12122017_Ct.csv</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>HD_63</t>
-  </si>
-  <si>
     <t>Warning</t>
   </si>
   <si>
-    <t>HD_32</t>
-  </si>
-  <si>
-    <t>HD_50</t>
-  </si>
-  <si>
     <t>LOD</t>
   </si>
   <si>
     <t>Missing Data freq.</t>
+  </si>
+  <si>
+    <t>CM-TEST-PA01-A1</t>
+  </si>
+  <si>
+    <t>CM-TEST-PA02-A1</t>
+  </si>
+  <si>
+    <t>CM-TEST-PA03-A1</t>
+  </si>
+  <si>
+    <t>CM-TEST-PA04-A1</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -922,6 +922,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -951,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -959,6 +964,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1276,7 +1282,7 @@
   <dimension ref="A1:CQ15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2434,8 +2440,8 @@
       </c>
     </row>
     <row r="9" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>286</v>
+      <c r="A9" s="7" t="s">
+        <v>291</v>
       </c>
       <c r="B9" s="2">
         <v>6.4387400000000001</v>
@@ -2711,15 +2717,15 @@
         <v>6.1181400000000004</v>
       </c>
       <c r="CP9" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ9" t="s">
         <v>287</v>
-      </c>
-      <c r="CQ9" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>289</v>
+      <c r="A10" s="7" t="s">
+        <v>292</v>
       </c>
       <c r="B10" s="4">
         <v>7.4578600000000002</v>
@@ -2995,15 +3001,15 @@
         <v>6.0998099999999997</v>
       </c>
       <c r="CP10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="CQ10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>291</v>
+      <c r="A11" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="B11" s="2">
         <v>5.3890399999999996</v>
@@ -3279,15 +3285,15 @@
         <v>5.9447799999999997</v>
       </c>
       <c r="CP11" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ11" t="s">
         <v>287</v>
-      </c>
-      <c r="CQ11" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>292</v>
+      <c r="A12" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="B12" s="2">
         <v>10.158770000000001</v>
@@ -3563,15 +3569,15 @@
         <v>5.9912700000000001</v>
       </c>
       <c r="CP12" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ12" t="s">
         <v>287</v>
-      </c>
-      <c r="CQ12" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B14" s="2">
         <v>1.2452799999999999</v>
@@ -3849,7 +3855,7 @@
     </row>
     <row r="15" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B15" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
Load CIMAC ID pattern from schema
</commit_message>
<xml_diff>
--- a/tests/data/olink/olink_assay_1_NPX.xlsx
+++ b/tests/data/olink/olink_assay_1_NPX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/tests/data/olink/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/tests/data/olink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC773223-16F1-4442-887B-4E67AA62E4CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFF1FF0-8556-E947-BACC-3A766B552A1E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="296">
   <si>
     <t>Olink NPX Manager 0.0.82.0</t>
   </si>
@@ -905,6 +905,9 @@
   </si>
   <si>
     <t>CTTTP04A1.00</t>
+  </si>
+  <si>
+    <t>non-cimac-control</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CQ15"/>
+  <dimension ref="A1:CQ16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3015,7 +3018,7 @@
     </row>
     <row r="11" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B11" s="2">
         <v>5.3890399999999996</v>
@@ -3298,281 +3301,281 @@
       </c>
     </row>
     <row r="12" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>294</v>
+      <c r="A12" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="B12" s="2">
-        <v>10.158770000000001</v>
+        <v>5.3890399999999996</v>
       </c>
       <c r="C12" s="2">
-        <v>7.4727499999999996</v>
-      </c>
-      <c r="E12" s="2">
-        <v>7.4537000000000004</v>
-      </c>
-      <c r="F12" s="2">
-        <v>7.3738299999999999</v>
+        <v>8.0275999999999996</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.64015</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.77817</v>
       </c>
       <c r="G12" s="2">
-        <v>5.9239600000000001</v>
+        <v>1.5354699999999999</v>
       </c>
       <c r="H12" s="2">
-        <v>7.4272499999999999</v>
+        <v>5.6791499999999999</v>
       </c>
       <c r="I12" s="2">
-        <v>6.1239100000000004</v>
+        <v>4.5099400000000003</v>
       </c>
       <c r="J12" s="2">
-        <v>8.5286899999999992</v>
+        <v>8.6995000000000005</v>
       </c>
       <c r="K12" s="2">
-        <v>6.2963199999999997</v>
+        <v>7.5098700000000003</v>
       </c>
       <c r="L12" s="2">
-        <v>8.7127300000000005</v>
+        <v>9.2407800000000009</v>
       </c>
       <c r="M12" s="2">
-        <v>10.038259999999999</v>
-      </c>
-      <c r="N12" s="2">
-        <v>8.3004899999999999</v>
+        <v>1.99051</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1.5549299999999999</v>
       </c>
       <c r="O12" s="2">
-        <v>9.3532299999999999</v>
-      </c>
-      <c r="P12" s="2">
-        <v>6.5704200000000004</v>
+        <v>8.1010600000000004</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1.0474699999999999</v>
       </c>
       <c r="Q12" s="2">
-        <v>9.1646699999999992</v>
+        <v>8.6572800000000001</v>
       </c>
       <c r="R12" s="2">
-        <v>6.2262199999999996</v>
+        <v>7.39635</v>
       </c>
       <c r="S12" s="2">
-        <v>7.17774</v>
-      </c>
-      <c r="T12" s="2">
-        <v>6.3941800000000004</v>
+        <v>6.5392099999999997</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0.96518000000000004</v>
       </c>
       <c r="U12" s="2">
-        <v>6.9149000000000003</v>
+        <v>5.6234900000000003</v>
       </c>
       <c r="V12" s="2">
-        <v>5.8858800000000002</v>
-      </c>
-      <c r="W12" s="2">
-        <v>7.5102500000000001</v>
-      </c>
-      <c r="X12" s="2">
-        <v>3.80145</v>
+        <v>5.19747</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1.67276</v>
+      </c>
+      <c r="X12" s="3">
+        <v>-0.73333000000000004</v>
       </c>
       <c r="Y12" s="2">
-        <v>4.8563599999999996</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>5.9795199999999999</v>
+        <v>1.1449800000000001</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>1.7403200000000001</v>
       </c>
       <c r="AA12" s="2">
-        <v>9.2229299999999999</v>
-      </c>
-      <c r="AB12" s="2">
-        <v>9.2211099999999995</v>
+        <v>9.2596299999999996</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>1.9816100000000001</v>
       </c>
       <c r="AC12" s="2">
-        <v>8.3966899999999995</v>
+        <v>5.0481600000000002</v>
       </c>
       <c r="AD12" s="2">
-        <v>7.4177499999999998</v>
+        <v>3.5706799999999999</v>
       </c>
       <c r="AE12" s="2">
-        <v>8.1916600000000006</v>
+        <v>8.8241099999999992</v>
       </c>
       <c r="AF12" s="2">
-        <v>6.0623300000000002</v>
+        <v>6.5130800000000004</v>
       </c>
       <c r="AG12" s="2">
-        <v>9.1206700000000005</v>
+        <v>1.70407</v>
       </c>
       <c r="AH12" s="2">
-        <v>6.2064899999999996</v>
+        <v>1.5643199999999999</v>
       </c>
       <c r="AI12" s="2">
-        <v>3.12277</v>
+        <v>4.62066</v>
       </c>
       <c r="AJ12" s="2">
-        <v>7.13347</v>
+        <v>6.0664400000000001</v>
       </c>
       <c r="AK12" s="2">
-        <v>5.5058299999999996</v>
+        <v>4.3881899999999998</v>
       </c>
       <c r="AL12" s="2">
-        <v>6.57064</v>
+        <v>1.6679999999999999</v>
       </c>
       <c r="AM12" s="2">
-        <v>5.57456</v>
-      </c>
-      <c r="AN12" s="2">
-        <v>5.6974900000000002</v>
+        <v>0.49991000000000002</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>1.2237499999999999</v>
       </c>
       <c r="AO12" s="2">
-        <v>10.532019999999999</v>
+        <v>14.24718</v>
       </c>
       <c r="AP12" s="2">
-        <v>4.6502100000000004</v>
+        <v>1.64514</v>
       </c>
       <c r="AQ12" s="2">
-        <v>5.2417499999999997</v>
+        <v>2.5803699999999998</v>
       </c>
       <c r="AR12" s="2">
-        <v>7.7904299999999997</v>
+        <v>7.4511900000000004</v>
       </c>
       <c r="AS12" s="2">
-        <v>4.2834199999999996</v>
+        <v>0.42118</v>
       </c>
       <c r="AT12" s="2">
-        <v>6.7729100000000004</v>
-      </c>
-      <c r="AU12" s="2">
-        <v>8.7543600000000001</v>
+        <v>5.1055000000000001</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>2.3804400000000001</v>
       </c>
       <c r="AV12" s="2">
-        <v>6.0541999999999998</v>
+        <v>5.0037399999999996</v>
       </c>
       <c r="AW12" s="2">
-        <v>8.0451899999999998</v>
+        <v>3.4083899999999998</v>
       </c>
       <c r="AX12" s="2">
-        <v>5.39635</v>
+        <v>1.0848</v>
       </c>
       <c r="AY12" s="2">
-        <v>10.5456</v>
+        <v>12.60385</v>
       </c>
       <c r="AZ12" s="2">
-        <v>7.3565100000000001</v>
+        <v>4.0495000000000001</v>
       </c>
       <c r="BA12" s="2">
-        <v>6.7207600000000003</v>
+        <v>6.5603400000000001</v>
       </c>
       <c r="BB12" s="2">
-        <v>3.4305500000000002</v>
-      </c>
-      <c r="BC12" s="2">
-        <v>9.7064699999999995</v>
-      </c>
-      <c r="BD12" s="2">
-        <v>6.1847399999999997</v>
-      </c>
-      <c r="BE12" s="2">
-        <v>5.1341099999999997</v>
+        <v>2.0788799999999998</v>
+      </c>
+      <c r="BC12" s="3">
+        <v>2.3016700000000001</v>
+      </c>
+      <c r="BD12" s="3">
+        <v>1.32935</v>
+      </c>
+      <c r="BE12" s="3">
+        <v>1.3167599999999999</v>
       </c>
       <c r="BF12" s="2">
-        <v>5.9257099999999996</v>
+        <v>5.7244900000000003</v>
       </c>
       <c r="BG12" s="2">
-        <v>6.2577100000000003</v>
-      </c>
-      <c r="BH12" s="2">
-        <v>7.2429300000000003</v>
+        <v>2.21645</v>
+      </c>
+      <c r="BH12" s="3">
+        <v>0.92159000000000002</v>
       </c>
       <c r="BI12" s="2">
-        <v>7.8703099999999999</v>
+        <v>6.7986000000000004</v>
       </c>
       <c r="BJ12" s="2">
-        <v>5.3787099999999999</v>
+        <v>4.2192499999999997</v>
       </c>
       <c r="BK12" s="2">
-        <v>8.0756599999999992</v>
+        <v>3.0885799999999999</v>
       </c>
       <c r="BL12" s="2">
-        <v>8.9649199999999993</v>
+        <v>6.6686100000000001</v>
       </c>
       <c r="BM12" s="2">
-        <v>7.9430699999999996</v>
+        <v>8.3308599999999995</v>
       </c>
       <c r="BN12" s="2">
-        <v>8.7584700000000009</v>
+        <v>7.6117800000000004</v>
       </c>
       <c r="BO12" s="2">
-        <v>6.3030999999999997</v>
-      </c>
-      <c r="BP12" s="2">
-        <v>6.1244800000000001</v>
+        <v>9.0845699999999994</v>
+      </c>
+      <c r="BP12" s="3">
+        <v>0.99180999999999997</v>
       </c>
       <c r="BQ12" s="2">
-        <v>6.0146199999999999</v>
+        <v>6.4739800000000001</v>
       </c>
       <c r="BR12" s="2">
-        <v>6.3564400000000001</v>
+        <v>1.50126</v>
       </c>
       <c r="BS12" s="2">
-        <v>6.6078400000000004</v>
+        <v>6.65564</v>
       </c>
       <c r="BT12" s="2">
-        <v>5.93649</v>
+        <v>2.8513899999999999</v>
       </c>
       <c r="BU12" s="2">
-        <v>8.8595600000000001</v>
-      </c>
-      <c r="BV12" s="2">
-        <v>6.8673400000000004</v>
-      </c>
-      <c r="BW12" s="2">
-        <v>6.3774600000000001</v>
+        <v>11.17624</v>
+      </c>
+      <c r="BV12" s="3">
+        <v>1.8282700000000001</v>
+      </c>
+      <c r="BW12" s="3">
+        <v>0.92803000000000002</v>
       </c>
       <c r="BX12" s="2">
-        <v>6.64602</v>
-      </c>
-      <c r="BY12" s="2">
-        <v>7.3281200000000002</v>
-      </c>
-      <c r="BZ12" s="2">
-        <v>7.0018399999999996</v>
-      </c>
-      <c r="CA12" s="2">
-        <v>6.7076700000000002</v>
+        <v>7.9254499999999997</v>
+      </c>
+      <c r="BY12" s="3">
+        <v>1.1127899999999999</v>
+      </c>
+      <c r="BZ12" s="3">
+        <v>0.83070999999999995</v>
+      </c>
+      <c r="CA12" s="3">
+        <v>0.71570999999999996</v>
       </c>
       <c r="CB12" s="2">
-        <v>8.1388599999999993</v>
+        <v>8.8757099999999998</v>
       </c>
       <c r="CC12" s="2">
-        <v>4.6814900000000002</v>
+        <v>3.8277399999999999</v>
       </c>
       <c r="CD12" s="2">
-        <v>6.4156700000000004</v>
+        <v>4.0646599999999999</v>
       </c>
       <c r="CE12" s="2">
-        <v>8.4468200000000007</v>
+        <v>4.6546200000000004</v>
       </c>
       <c r="CF12" s="2">
-        <v>7.7824900000000001</v>
+        <v>4.7480599999999997</v>
       </c>
       <c r="CG12" s="2">
-        <v>6.5670400000000004</v>
+        <v>1.39032</v>
       </c>
       <c r="CH12" s="2">
-        <v>9.1699900000000003</v>
+        <v>8.7408900000000003</v>
       </c>
       <c r="CI12" s="2">
-        <v>8.5052800000000008</v>
+        <v>5.4637700000000002</v>
       </c>
       <c r="CJ12" s="2">
-        <v>5.9825299999999997</v>
+        <v>5.5136500000000002</v>
       </c>
       <c r="CK12" s="2">
-        <v>5.9964899999999997</v>
+        <v>8.0868500000000001</v>
       </c>
       <c r="CL12" s="2">
-        <v>6.9250800000000003</v>
+        <v>2.0654499999999998</v>
       </c>
       <c r="CM12" s="2">
-        <v>6.49444</v>
+        <v>3.9321600000000001</v>
       </c>
       <c r="CN12" s="2">
-        <v>6.3431699999999998</v>
+        <v>2.5042300000000002</v>
       </c>
       <c r="CO12" s="2">
-        <v>5.9912700000000001</v>
+        <v>5.9447799999999997</v>
       </c>
       <c r="CP12" t="s">
         <v>286</v>
@@ -3581,562 +3584,846 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.2452799999999999</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.73102</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1.64015</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1.77817</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.56850000000000001</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1.76467</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.79384999999999994</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.73258000000000001</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1.22241</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1.2118100000000001</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1.1236699999999999</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1.5549299999999999</v>
-      </c>
-      <c r="O14" s="2">
-        <v>1.11277</v>
-      </c>
-      <c r="P14" s="2">
-        <v>1.0474699999999999</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0.99802000000000002</v>
-      </c>
-      <c r="R14" s="2">
-        <v>1.3523400000000001</v>
-      </c>
-      <c r="S14" s="2">
-        <v>1.0710900000000001</v>
-      </c>
-      <c r="T14" s="2">
-        <v>0.96518000000000004</v>
-      </c>
-      <c r="U14" s="2">
-        <v>0.94247000000000003</v>
-      </c>
-      <c r="V14" s="2">
-        <v>-1.06471</v>
-      </c>
-      <c r="W14" s="2">
-        <v>1.67276</v>
-      </c>
-      <c r="X14" s="2">
-        <v>-0.73333000000000004</v>
-      </c>
-      <c r="Y14" s="2">
-        <v>0.73509000000000002</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>1.7403200000000001</v>
-      </c>
-      <c r="AA14" s="2">
-        <v>2.56996</v>
-      </c>
-      <c r="AB14" s="2">
-        <v>1.9816100000000001</v>
-      </c>
-      <c r="AC14" s="2">
-        <v>1.64662</v>
-      </c>
-      <c r="AD14" s="2">
-        <v>1.1802600000000001</v>
-      </c>
-      <c r="AE14" s="2">
-        <v>1.7056500000000001</v>
-      </c>
-      <c r="AF14" s="2">
-        <v>1.34832</v>
-      </c>
-      <c r="AG14" s="2">
-        <v>0.95889999999999997</v>
-      </c>
-      <c r="AH14" s="2">
-        <v>1.1231899999999999</v>
-      </c>
-      <c r="AI14" s="2">
-        <v>-0.39773999999999998</v>
-      </c>
-      <c r="AJ14" s="2">
-        <v>0.92922000000000005</v>
-      </c>
-      <c r="AK14" s="2">
-        <v>1.2955399999999999</v>
-      </c>
-      <c r="AL14" s="2">
-        <v>1.6230800000000001</v>
-      </c>
-      <c r="AM14" s="2">
-        <v>0.37853999999999999</v>
-      </c>
-      <c r="AN14" s="2">
-        <v>1.2237499999999999</v>
-      </c>
-      <c r="AO14" s="2">
-        <v>1.11005</v>
-      </c>
-      <c r="AP14" s="2">
-        <v>1.1332500000000001</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>0.82589000000000001</v>
-      </c>
-      <c r="AR14" s="2">
-        <v>1.4808399999999999</v>
-      </c>
-      <c r="AS14" s="2">
-        <v>0.33593000000000001</v>
-      </c>
-      <c r="AT14" s="2">
-        <v>0.68486000000000002</v>
-      </c>
-      <c r="AU14" s="2">
-        <v>2.3804400000000001</v>
-      </c>
-      <c r="AV14" s="2">
-        <v>1.5673699999999999</v>
-      </c>
-      <c r="AW14" s="2">
-        <v>2.2438500000000001</v>
-      </c>
-      <c r="AX14" s="2">
-        <v>0.68201999999999996</v>
-      </c>
-      <c r="AY14" s="2">
-        <v>1.80481</v>
-      </c>
-      <c r="AZ14" s="2">
-        <v>1.67354</v>
-      </c>
-      <c r="BA14" s="2">
-        <v>1.2162599999999999</v>
-      </c>
-      <c r="BB14" s="2">
-        <v>0.36577999999999999</v>
-      </c>
-      <c r="BC14" s="2">
-        <v>2.3016700000000001</v>
-      </c>
-      <c r="BD14" s="2">
-        <v>1.32935</v>
-      </c>
-      <c r="BE14" s="2">
-        <v>1.3167599999999999</v>
-      </c>
-      <c r="BF14" s="2">
-        <v>0.98580000000000001</v>
-      </c>
-      <c r="BG14" s="2">
-        <v>1.6696899999999999</v>
-      </c>
-      <c r="BH14" s="2">
-        <v>0.92159000000000002</v>
-      </c>
-      <c r="BI14" s="2">
-        <v>1.08039</v>
-      </c>
-      <c r="BJ14" s="2">
-        <v>0.75095000000000001</v>
-      </c>
-      <c r="BK14" s="2">
-        <v>1.3260799999999999</v>
-      </c>
-      <c r="BL14" s="2">
-        <v>2.1433499999999999</v>
-      </c>
-      <c r="BM14" s="2">
-        <v>0.89825999999999995</v>
-      </c>
-      <c r="BN14" s="2">
-        <v>2.4283100000000002</v>
-      </c>
-      <c r="BO14" s="2">
-        <v>1.12523</v>
-      </c>
-      <c r="BP14" s="2">
-        <v>0.99180999999999997</v>
-      </c>
-      <c r="BQ14" s="2">
-        <v>2.07457</v>
-      </c>
-      <c r="BR14" s="2">
-        <v>1.1291800000000001</v>
-      </c>
-      <c r="BS14" s="2">
-        <v>0.65888999999999998</v>
-      </c>
-      <c r="BT14" s="2">
-        <v>0.68162999999999996</v>
-      </c>
-      <c r="BU14" s="2">
-        <v>1.9415</v>
-      </c>
-      <c r="BV14" s="2">
-        <v>1.8282700000000001</v>
-      </c>
-      <c r="BW14" s="2">
-        <v>0.92803000000000002</v>
-      </c>
-      <c r="BX14" s="2">
-        <v>1.3465199999999999</v>
-      </c>
-      <c r="BY14" s="2">
-        <v>1.1127899999999999</v>
-      </c>
-      <c r="BZ14" s="2">
-        <v>0.83070999999999995</v>
-      </c>
-      <c r="CA14" s="2">
-        <v>0.71570999999999996</v>
-      </c>
-      <c r="CB14" s="2">
-        <v>1.8677600000000001</v>
-      </c>
-      <c r="CC14" s="2">
-        <v>1.6599900000000001</v>
-      </c>
-      <c r="CD14" s="2">
-        <v>0.65619000000000005</v>
-      </c>
-      <c r="CE14" s="2">
-        <v>1.6655899999999999</v>
-      </c>
-      <c r="CF14" s="2">
-        <v>1.9583999999999999</v>
-      </c>
-      <c r="CG14" s="2">
-        <v>1.26908</v>
-      </c>
-      <c r="CH14" s="2">
-        <v>1.97288</v>
-      </c>
-      <c r="CI14" s="2">
-        <v>1.7742500000000001</v>
-      </c>
-      <c r="CJ14" s="2">
-        <v>0.85163</v>
-      </c>
-      <c r="CK14" s="2">
-        <v>1.5718799999999999</v>
-      </c>
-      <c r="CL14" s="2">
-        <v>1.7406600000000001</v>
-      </c>
-      <c r="CM14" s="2">
-        <v>1.2820499999999999</v>
-      </c>
-      <c r="CN14" s="2">
-        <v>1.3283700000000001</v>
-      </c>
-      <c r="CO14" s="2">
-        <v>1.49448</v>
+    <row r="13" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10.158770000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.4727499999999996</v>
+      </c>
+      <c r="E13" s="2">
+        <v>7.4537000000000004</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.3738299999999999</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.9239600000000001</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7.4272499999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.1239100000000004</v>
+      </c>
+      <c r="J13" s="2">
+        <v>8.5286899999999992</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6.2963199999999997</v>
+      </c>
+      <c r="L13" s="2">
+        <v>8.7127300000000005</v>
+      </c>
+      <c r="M13" s="2">
+        <v>10.038259999999999</v>
+      </c>
+      <c r="N13" s="2">
+        <v>8.3004899999999999</v>
+      </c>
+      <c r="O13" s="2">
+        <v>9.3532299999999999</v>
+      </c>
+      <c r="P13" s="2">
+        <v>6.5704200000000004</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>9.1646699999999992</v>
+      </c>
+      <c r="R13" s="2">
+        <v>6.2262199999999996</v>
+      </c>
+      <c r="S13" s="2">
+        <v>7.17774</v>
+      </c>
+      <c r="T13" s="2">
+        <v>6.3941800000000004</v>
+      </c>
+      <c r="U13" s="2">
+        <v>6.9149000000000003</v>
+      </c>
+      <c r="V13" s="2">
+        <v>5.8858800000000002</v>
+      </c>
+      <c r="W13" s="2">
+        <v>7.5102500000000001</v>
+      </c>
+      <c r="X13" s="2">
+        <v>3.80145</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>4.8563599999999996</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>5.9795199999999999</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>9.2229299999999999</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>9.2211099999999995</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>8.3966899999999995</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>7.4177499999999998</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>8.1916600000000006</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>6.0623300000000002</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>9.1206700000000005</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>6.2064899999999996</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>3.12277</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>7.13347</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>5.5058299999999996</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>6.57064</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>5.57456</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>5.6974900000000002</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>10.532019999999999</v>
+      </c>
+      <c r="AP13" s="2">
+        <v>4.6502100000000004</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>5.2417499999999997</v>
+      </c>
+      <c r="AR13" s="2">
+        <v>7.7904299999999997</v>
+      </c>
+      <c r="AS13" s="2">
+        <v>4.2834199999999996</v>
+      </c>
+      <c r="AT13" s="2">
+        <v>6.7729100000000004</v>
+      </c>
+      <c r="AU13" s="2">
+        <v>8.7543600000000001</v>
+      </c>
+      <c r="AV13" s="2">
+        <v>6.0541999999999998</v>
+      </c>
+      <c r="AW13" s="2">
+        <v>8.0451899999999998</v>
+      </c>
+      <c r="AX13" s="2">
+        <v>5.39635</v>
+      </c>
+      <c r="AY13" s="2">
+        <v>10.5456</v>
+      </c>
+      <c r="AZ13" s="2">
+        <v>7.3565100000000001</v>
+      </c>
+      <c r="BA13" s="2">
+        <v>6.7207600000000003</v>
+      </c>
+      <c r="BB13" s="2">
+        <v>3.4305500000000002</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>9.7064699999999995</v>
+      </c>
+      <c r="BD13" s="2">
+        <v>6.1847399999999997</v>
+      </c>
+      <c r="BE13" s="2">
+        <v>5.1341099999999997</v>
+      </c>
+      <c r="BF13" s="2">
+        <v>5.9257099999999996</v>
+      </c>
+      <c r="BG13" s="2">
+        <v>6.2577100000000003</v>
+      </c>
+      <c r="BH13" s="2">
+        <v>7.2429300000000003</v>
+      </c>
+      <c r="BI13" s="2">
+        <v>7.8703099999999999</v>
+      </c>
+      <c r="BJ13" s="2">
+        <v>5.3787099999999999</v>
+      </c>
+      <c r="BK13" s="2">
+        <v>8.0756599999999992</v>
+      </c>
+      <c r="BL13" s="2">
+        <v>8.9649199999999993</v>
+      </c>
+      <c r="BM13" s="2">
+        <v>7.9430699999999996</v>
+      </c>
+      <c r="BN13" s="2">
+        <v>8.7584700000000009</v>
+      </c>
+      <c r="BO13" s="2">
+        <v>6.3030999999999997</v>
+      </c>
+      <c r="BP13" s="2">
+        <v>6.1244800000000001</v>
+      </c>
+      <c r="BQ13" s="2">
+        <v>6.0146199999999999</v>
+      </c>
+      <c r="BR13" s="2">
+        <v>6.3564400000000001</v>
+      </c>
+      <c r="BS13" s="2">
+        <v>6.6078400000000004</v>
+      </c>
+      <c r="BT13" s="2">
+        <v>5.93649</v>
+      </c>
+      <c r="BU13" s="2">
+        <v>8.8595600000000001</v>
+      </c>
+      <c r="BV13" s="2">
+        <v>6.8673400000000004</v>
+      </c>
+      <c r="BW13" s="2">
+        <v>6.3774600000000001</v>
+      </c>
+      <c r="BX13" s="2">
+        <v>6.64602</v>
+      </c>
+      <c r="BY13" s="2">
+        <v>7.3281200000000002</v>
+      </c>
+      <c r="BZ13" s="2">
+        <v>7.0018399999999996</v>
+      </c>
+      <c r="CA13" s="2">
+        <v>6.7076700000000002</v>
+      </c>
+      <c r="CB13" s="2">
+        <v>8.1388599999999993</v>
+      </c>
+      <c r="CC13" s="2">
+        <v>4.6814900000000002</v>
+      </c>
+      <c r="CD13" s="2">
+        <v>6.4156700000000004</v>
+      </c>
+      <c r="CE13" s="2">
+        <v>8.4468200000000007</v>
+      </c>
+      <c r="CF13" s="2">
+        <v>7.7824900000000001</v>
+      </c>
+      <c r="CG13" s="2">
+        <v>6.5670400000000004</v>
+      </c>
+      <c r="CH13" s="2">
+        <v>9.1699900000000003</v>
+      </c>
+      <c r="CI13" s="2">
+        <v>8.5052800000000008</v>
+      </c>
+      <c r="CJ13" s="2">
+        <v>5.9825299999999997</v>
+      </c>
+      <c r="CK13" s="2">
+        <v>5.9964899999999997</v>
+      </c>
+      <c r="CL13" s="2">
+        <v>6.9250800000000003</v>
+      </c>
+      <c r="CM13" s="2">
+        <v>6.49444</v>
+      </c>
+      <c r="CN13" s="2">
+        <v>6.3431699999999998</v>
+      </c>
+      <c r="CO13" s="2">
+        <v>5.9912700000000001</v>
+      </c>
+      <c r="CP13" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ13" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.2452799999999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.73102</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.64015</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.77817</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.56850000000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.76467</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.79384999999999994</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.73258000000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.22241</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.2118100000000001</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.1236699999999999</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.5549299999999999</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.11277</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1.0474699999999999</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0.99802000000000002</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1.3523400000000001</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.0710900000000001</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0.96518000000000004</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0.94247000000000003</v>
+      </c>
+      <c r="V15" s="2">
+        <v>-1.06471</v>
+      </c>
+      <c r="W15" s="2">
+        <v>1.67276</v>
+      </c>
+      <c r="X15" s="2">
+        <v>-0.73333000000000004</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0.73509000000000002</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1.7403200000000001</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>2.56996</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>1.9816100000000001</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>1.64662</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>1.1802600000000001</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>1.7056500000000001</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>1.34832</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>0.95889999999999997</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>1.1231899999999999</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>-0.39773999999999998</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>0.92922000000000005</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>1.2955399999999999</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>1.6230800000000001</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>0.37853999999999999</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>1.2237499999999999</v>
+      </c>
+      <c r="AO15" s="2">
+        <v>1.11005</v>
+      </c>
+      <c r="AP15" s="2">
+        <v>1.1332500000000001</v>
+      </c>
+      <c r="AQ15" s="2">
+        <v>0.82589000000000001</v>
+      </c>
+      <c r="AR15" s="2">
+        <v>1.4808399999999999</v>
+      </c>
+      <c r="AS15" s="2">
+        <v>0.33593000000000001</v>
+      </c>
+      <c r="AT15" s="2">
+        <v>0.68486000000000002</v>
+      </c>
+      <c r="AU15" s="2">
+        <v>2.3804400000000001</v>
+      </c>
+      <c r="AV15" s="2">
+        <v>1.5673699999999999</v>
+      </c>
+      <c r="AW15" s="2">
+        <v>2.2438500000000001</v>
+      </c>
+      <c r="AX15" s="2">
+        <v>0.68201999999999996</v>
+      </c>
+      <c r="AY15" s="2">
+        <v>1.80481</v>
+      </c>
+      <c r="AZ15" s="2">
+        <v>1.67354</v>
+      </c>
+      <c r="BA15" s="2">
+        <v>1.2162599999999999</v>
+      </c>
+      <c r="BB15" s="2">
+        <v>0.36577999999999999</v>
+      </c>
+      <c r="BC15" s="2">
+        <v>2.3016700000000001</v>
+      </c>
+      <c r="BD15" s="2">
+        <v>1.32935</v>
+      </c>
+      <c r="BE15" s="2">
+        <v>1.3167599999999999</v>
+      </c>
+      <c r="BF15" s="2">
+        <v>0.98580000000000001</v>
+      </c>
+      <c r="BG15" s="2">
+        <v>1.6696899999999999</v>
+      </c>
+      <c r="BH15" s="2">
+        <v>0.92159000000000002</v>
+      </c>
+      <c r="BI15" s="2">
+        <v>1.08039</v>
+      </c>
+      <c r="BJ15" s="2">
+        <v>0.75095000000000001</v>
+      </c>
+      <c r="BK15" s="2">
+        <v>1.3260799999999999</v>
+      </c>
+      <c r="BL15" s="2">
+        <v>2.1433499999999999</v>
+      </c>
+      <c r="BM15" s="2">
+        <v>0.89825999999999995</v>
+      </c>
+      <c r="BN15" s="2">
+        <v>2.4283100000000002</v>
+      </c>
+      <c r="BO15" s="2">
+        <v>1.12523</v>
+      </c>
+      <c r="BP15" s="2">
+        <v>0.99180999999999997</v>
+      </c>
+      <c r="BQ15" s="2">
+        <v>2.07457</v>
+      </c>
+      <c r="BR15" s="2">
+        <v>1.1291800000000001</v>
+      </c>
+      <c r="BS15" s="2">
+        <v>0.65888999999999998</v>
+      </c>
+      <c r="BT15" s="2">
+        <v>0.68162999999999996</v>
+      </c>
+      <c r="BU15" s="2">
+        <v>1.9415</v>
+      </c>
+      <c r="BV15" s="2">
+        <v>1.8282700000000001</v>
+      </c>
+      <c r="BW15" s="2">
+        <v>0.92803000000000002</v>
+      </c>
+      <c r="BX15" s="2">
+        <v>1.3465199999999999</v>
+      </c>
+      <c r="BY15" s="2">
+        <v>1.1127899999999999</v>
+      </c>
+      <c r="BZ15" s="2">
+        <v>0.83070999999999995</v>
+      </c>
+      <c r="CA15" s="2">
+        <v>0.71570999999999996</v>
+      </c>
+      <c r="CB15" s="2">
+        <v>1.8677600000000001</v>
+      </c>
+      <c r="CC15" s="2">
+        <v>1.6599900000000001</v>
+      </c>
+      <c r="CD15" s="2">
+        <v>0.65619000000000005</v>
+      </c>
+      <c r="CE15" s="2">
+        <v>1.6655899999999999</v>
+      </c>
+      <c r="CF15" s="2">
+        <v>1.9583999999999999</v>
+      </c>
+      <c r="CG15" s="2">
+        <v>1.26908</v>
+      </c>
+      <c r="CH15" s="2">
+        <v>1.97288</v>
+      </c>
+      <c r="CI15" s="2">
+        <v>1.7742500000000001</v>
+      </c>
+      <c r="CJ15" s="2">
+        <v>0.85163</v>
+      </c>
+      <c r="CK15" s="2">
+        <v>1.5718799999999999</v>
+      </c>
+      <c r="CL15" s="2">
+        <v>1.7406600000000001</v>
+      </c>
+      <c r="CM15" s="2">
+        <v>1.2820499999999999</v>
+      </c>
+      <c r="CN15" s="2">
+        <v>1.3283700000000001</v>
+      </c>
+      <c r="CO15" s="2">
+        <v>1.49448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>290</v>
       </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E16" s="6">
         <v>0.25</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F16" s="6">
         <v>0.75</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
-        <v>0</v>
-      </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
         <v>0.5</v>
       </c>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="P15" s="6">
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
         <v>0.75</v>
       </c>
-      <c r="Q15" s="6">
-        <v>0</v>
-      </c>
-      <c r="R15" s="6">
-        <v>0</v>
-      </c>
-      <c r="S15" s="6">
-        <v>0</v>
-      </c>
-      <c r="T15" s="6">
+      <c r="Q16" s="6">
+        <v>0</v>
+      </c>
+      <c r="R16" s="6">
+        <v>0</v>
+      </c>
+      <c r="S16" s="6">
+        <v>0</v>
+      </c>
+      <c r="T16" s="6">
         <v>0.75</v>
       </c>
-      <c r="U15" s="6">
-        <v>0</v>
-      </c>
-      <c r="V15" s="6">
-        <v>0</v>
-      </c>
-      <c r="W15" s="6">
+      <c r="U16" s="6">
+        <v>0</v>
+      </c>
+      <c r="V16" s="6">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6">
         <v>0.75</v>
       </c>
-      <c r="X15" s="6">
+      <c r="X16" s="6">
         <v>0.75</v>
       </c>
-      <c r="Y15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="6">
+      <c r="Y16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AA15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="6">
+      <c r="AA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AC15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="6">
+      <c r="AC16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="6">
         <v>0.25</v>
       </c>
-      <c r="AH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="6">
+      <c r="AH16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="6">
         <v>0.25</v>
       </c>
-      <c r="AM15" s="6">
+      <c r="AM16" s="6">
         <v>0.5</v>
       </c>
-      <c r="AN15" s="6">
+      <c r="AN16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AO15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS15" s="6">
+      <c r="AO16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="6">
         <v>0.5</v>
       </c>
-      <c r="AT15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AU15" s="6">
+      <c r="AT16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AV15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AW15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AX15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AY15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BA15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BB15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BC15" s="6">
+      <c r="AV16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AX16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BD15" s="6">
+      <c r="BD16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BE15" s="6">
+      <c r="BE16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BF15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BG15" s="6">
+      <c r="BF16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BG16" s="6">
         <v>0.25</v>
       </c>
-      <c r="BH15" s="6">
+      <c r="BH16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BI15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BJ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BL15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BM15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BN15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BO15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BP15" s="6">
+      <c r="BI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BK16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BM16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BN16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BO16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BP16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BQ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BR15" s="6">
+      <c r="BQ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BR16" s="6">
         <v>0.5</v>
       </c>
-      <c r="BS15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BT15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BU15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BV15" s="6">
+      <c r="BS16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BT16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BU16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BV16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BW15" s="6">
+      <c r="BW16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BX15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BY15" s="6">
+      <c r="BX16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BY16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BZ15" s="6">
+      <c r="BZ16" s="6">
         <v>0.75</v>
       </c>
-      <c r="CA15" s="6">
+      <c r="CA16" s="6">
         <v>0.75</v>
       </c>
-      <c r="CB15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CC15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CD15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CE15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CF15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CG15" s="6">
+      <c r="CB16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CC16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CD16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CE16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CF16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CG16" s="6">
         <v>0.25</v>
       </c>
-      <c r="CH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CI15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CJ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CL15" s="6">
+      <c r="CH16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CK16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CL16" s="6">
         <v>0.5</v>
       </c>
-      <c r="CM15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CN15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CO15" s="6">
+      <c r="CM16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CN16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CO16" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ignore non-CIMAC ids in NPX files (#211)
* Ignore non-CIMAC ids in NPX files

* Load CIMAC ID pattern from schema

* Bump package version
</commit_message>
<xml_diff>
--- a/tests/data/olink/olink_assay_1_NPX.xlsx
+++ b/tests/data/olink/olink_assay_1_NPX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/tests/data/olink/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/tests/data/olink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC773223-16F1-4442-887B-4E67AA62E4CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFF1FF0-8556-E947-BACC-3A766B552A1E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="296">
   <si>
     <t>Olink NPX Manager 0.0.82.0</t>
   </si>
@@ -905,6 +905,9 @@
   </si>
   <si>
     <t>CTTTP04A1.00</t>
+  </si>
+  <si>
+    <t>non-cimac-control</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CQ15"/>
+  <dimension ref="A1:CQ16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3015,7 +3018,7 @@
     </row>
     <row r="11" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B11" s="2">
         <v>5.3890399999999996</v>
@@ -3298,281 +3301,281 @@
       </c>
     </row>
     <row r="12" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>294</v>
+      <c r="A12" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="B12" s="2">
-        <v>10.158770000000001</v>
+        <v>5.3890399999999996</v>
       </c>
       <c r="C12" s="2">
-        <v>7.4727499999999996</v>
-      </c>
-      <c r="E12" s="2">
-        <v>7.4537000000000004</v>
-      </c>
-      <c r="F12" s="2">
-        <v>7.3738299999999999</v>
+        <v>8.0275999999999996</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.64015</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.77817</v>
       </c>
       <c r="G12" s="2">
-        <v>5.9239600000000001</v>
+        <v>1.5354699999999999</v>
       </c>
       <c r="H12" s="2">
-        <v>7.4272499999999999</v>
+        <v>5.6791499999999999</v>
       </c>
       <c r="I12" s="2">
-        <v>6.1239100000000004</v>
+        <v>4.5099400000000003</v>
       </c>
       <c r="J12" s="2">
-        <v>8.5286899999999992</v>
+        <v>8.6995000000000005</v>
       </c>
       <c r="K12" s="2">
-        <v>6.2963199999999997</v>
+        <v>7.5098700000000003</v>
       </c>
       <c r="L12" s="2">
-        <v>8.7127300000000005</v>
+        <v>9.2407800000000009</v>
       </c>
       <c r="M12" s="2">
-        <v>10.038259999999999</v>
-      </c>
-      <c r="N12" s="2">
-        <v>8.3004899999999999</v>
+        <v>1.99051</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1.5549299999999999</v>
       </c>
       <c r="O12" s="2">
-        <v>9.3532299999999999</v>
-      </c>
-      <c r="P12" s="2">
-        <v>6.5704200000000004</v>
+        <v>8.1010600000000004</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1.0474699999999999</v>
       </c>
       <c r="Q12" s="2">
-        <v>9.1646699999999992</v>
+        <v>8.6572800000000001</v>
       </c>
       <c r="R12" s="2">
-        <v>6.2262199999999996</v>
+        <v>7.39635</v>
       </c>
       <c r="S12" s="2">
-        <v>7.17774</v>
-      </c>
-      <c r="T12" s="2">
-        <v>6.3941800000000004</v>
+        <v>6.5392099999999997</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0.96518000000000004</v>
       </c>
       <c r="U12" s="2">
-        <v>6.9149000000000003</v>
+        <v>5.6234900000000003</v>
       </c>
       <c r="V12" s="2">
-        <v>5.8858800000000002</v>
-      </c>
-      <c r="W12" s="2">
-        <v>7.5102500000000001</v>
-      </c>
-      <c r="X12" s="2">
-        <v>3.80145</v>
+        <v>5.19747</v>
+      </c>
+      <c r="W12" s="3">
+        <v>1.67276</v>
+      </c>
+      <c r="X12" s="3">
+        <v>-0.73333000000000004</v>
       </c>
       <c r="Y12" s="2">
-        <v>4.8563599999999996</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>5.9795199999999999</v>
+        <v>1.1449800000000001</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>1.7403200000000001</v>
       </c>
       <c r="AA12" s="2">
-        <v>9.2229299999999999</v>
-      </c>
-      <c r="AB12" s="2">
-        <v>9.2211099999999995</v>
+        <v>9.2596299999999996</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>1.9816100000000001</v>
       </c>
       <c r="AC12" s="2">
-        <v>8.3966899999999995</v>
+        <v>5.0481600000000002</v>
       </c>
       <c r="AD12" s="2">
-        <v>7.4177499999999998</v>
+        <v>3.5706799999999999</v>
       </c>
       <c r="AE12" s="2">
-        <v>8.1916600000000006</v>
+        <v>8.8241099999999992</v>
       </c>
       <c r="AF12" s="2">
-        <v>6.0623300000000002</v>
+        <v>6.5130800000000004</v>
       </c>
       <c r="AG12" s="2">
-        <v>9.1206700000000005</v>
+        <v>1.70407</v>
       </c>
       <c r="AH12" s="2">
-        <v>6.2064899999999996</v>
+        <v>1.5643199999999999</v>
       </c>
       <c r="AI12" s="2">
-        <v>3.12277</v>
+        <v>4.62066</v>
       </c>
       <c r="AJ12" s="2">
-        <v>7.13347</v>
+        <v>6.0664400000000001</v>
       </c>
       <c r="AK12" s="2">
-        <v>5.5058299999999996</v>
+        <v>4.3881899999999998</v>
       </c>
       <c r="AL12" s="2">
-        <v>6.57064</v>
+        <v>1.6679999999999999</v>
       </c>
       <c r="AM12" s="2">
-        <v>5.57456</v>
-      </c>
-      <c r="AN12" s="2">
-        <v>5.6974900000000002</v>
+        <v>0.49991000000000002</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>1.2237499999999999</v>
       </c>
       <c r="AO12" s="2">
-        <v>10.532019999999999</v>
+        <v>14.24718</v>
       </c>
       <c r="AP12" s="2">
-        <v>4.6502100000000004</v>
+        <v>1.64514</v>
       </c>
       <c r="AQ12" s="2">
-        <v>5.2417499999999997</v>
+        <v>2.5803699999999998</v>
       </c>
       <c r="AR12" s="2">
-        <v>7.7904299999999997</v>
+        <v>7.4511900000000004</v>
       </c>
       <c r="AS12" s="2">
-        <v>4.2834199999999996</v>
+        <v>0.42118</v>
       </c>
       <c r="AT12" s="2">
-        <v>6.7729100000000004</v>
-      </c>
-      <c r="AU12" s="2">
-        <v>8.7543600000000001</v>
+        <v>5.1055000000000001</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>2.3804400000000001</v>
       </c>
       <c r="AV12" s="2">
-        <v>6.0541999999999998</v>
+        <v>5.0037399999999996</v>
       </c>
       <c r="AW12" s="2">
-        <v>8.0451899999999998</v>
+        <v>3.4083899999999998</v>
       </c>
       <c r="AX12" s="2">
-        <v>5.39635</v>
+        <v>1.0848</v>
       </c>
       <c r="AY12" s="2">
-        <v>10.5456</v>
+        <v>12.60385</v>
       </c>
       <c r="AZ12" s="2">
-        <v>7.3565100000000001</v>
+        <v>4.0495000000000001</v>
       </c>
       <c r="BA12" s="2">
-        <v>6.7207600000000003</v>
+        <v>6.5603400000000001</v>
       </c>
       <c r="BB12" s="2">
-        <v>3.4305500000000002</v>
-      </c>
-      <c r="BC12" s="2">
-        <v>9.7064699999999995</v>
-      </c>
-      <c r="BD12" s="2">
-        <v>6.1847399999999997</v>
-      </c>
-      <c r="BE12" s="2">
-        <v>5.1341099999999997</v>
+        <v>2.0788799999999998</v>
+      </c>
+      <c r="BC12" s="3">
+        <v>2.3016700000000001</v>
+      </c>
+      <c r="BD12" s="3">
+        <v>1.32935</v>
+      </c>
+      <c r="BE12" s="3">
+        <v>1.3167599999999999</v>
       </c>
       <c r="BF12" s="2">
-        <v>5.9257099999999996</v>
+        <v>5.7244900000000003</v>
       </c>
       <c r="BG12" s="2">
-        <v>6.2577100000000003</v>
-      </c>
-      <c r="BH12" s="2">
-        <v>7.2429300000000003</v>
+        <v>2.21645</v>
+      </c>
+      <c r="BH12" s="3">
+        <v>0.92159000000000002</v>
       </c>
       <c r="BI12" s="2">
-        <v>7.8703099999999999</v>
+        <v>6.7986000000000004</v>
       </c>
       <c r="BJ12" s="2">
-        <v>5.3787099999999999</v>
+        <v>4.2192499999999997</v>
       </c>
       <c r="BK12" s="2">
-        <v>8.0756599999999992</v>
+        <v>3.0885799999999999</v>
       </c>
       <c r="BL12" s="2">
-        <v>8.9649199999999993</v>
+        <v>6.6686100000000001</v>
       </c>
       <c r="BM12" s="2">
-        <v>7.9430699999999996</v>
+        <v>8.3308599999999995</v>
       </c>
       <c r="BN12" s="2">
-        <v>8.7584700000000009</v>
+        <v>7.6117800000000004</v>
       </c>
       <c r="BO12" s="2">
-        <v>6.3030999999999997</v>
-      </c>
-      <c r="BP12" s="2">
-        <v>6.1244800000000001</v>
+        <v>9.0845699999999994</v>
+      </c>
+      <c r="BP12" s="3">
+        <v>0.99180999999999997</v>
       </c>
       <c r="BQ12" s="2">
-        <v>6.0146199999999999</v>
+        <v>6.4739800000000001</v>
       </c>
       <c r="BR12" s="2">
-        <v>6.3564400000000001</v>
+        <v>1.50126</v>
       </c>
       <c r="BS12" s="2">
-        <v>6.6078400000000004</v>
+        <v>6.65564</v>
       </c>
       <c r="BT12" s="2">
-        <v>5.93649</v>
+        <v>2.8513899999999999</v>
       </c>
       <c r="BU12" s="2">
-        <v>8.8595600000000001</v>
-      </c>
-      <c r="BV12" s="2">
-        <v>6.8673400000000004</v>
-      </c>
-      <c r="BW12" s="2">
-        <v>6.3774600000000001</v>
+        <v>11.17624</v>
+      </c>
+      <c r="BV12" s="3">
+        <v>1.8282700000000001</v>
+      </c>
+      <c r="BW12" s="3">
+        <v>0.92803000000000002</v>
       </c>
       <c r="BX12" s="2">
-        <v>6.64602</v>
-      </c>
-      <c r="BY12" s="2">
-        <v>7.3281200000000002</v>
-      </c>
-      <c r="BZ12" s="2">
-        <v>7.0018399999999996</v>
-      </c>
-      <c r="CA12" s="2">
-        <v>6.7076700000000002</v>
+        <v>7.9254499999999997</v>
+      </c>
+      <c r="BY12" s="3">
+        <v>1.1127899999999999</v>
+      </c>
+      <c r="BZ12" s="3">
+        <v>0.83070999999999995</v>
+      </c>
+      <c r="CA12" s="3">
+        <v>0.71570999999999996</v>
       </c>
       <c r="CB12" s="2">
-        <v>8.1388599999999993</v>
+        <v>8.8757099999999998</v>
       </c>
       <c r="CC12" s="2">
-        <v>4.6814900000000002</v>
+        <v>3.8277399999999999</v>
       </c>
       <c r="CD12" s="2">
-        <v>6.4156700000000004</v>
+        <v>4.0646599999999999</v>
       </c>
       <c r="CE12" s="2">
-        <v>8.4468200000000007</v>
+        <v>4.6546200000000004</v>
       </c>
       <c r="CF12" s="2">
-        <v>7.7824900000000001</v>
+        <v>4.7480599999999997</v>
       </c>
       <c r="CG12" s="2">
-        <v>6.5670400000000004</v>
+        <v>1.39032</v>
       </c>
       <c r="CH12" s="2">
-        <v>9.1699900000000003</v>
+        <v>8.7408900000000003</v>
       </c>
       <c r="CI12" s="2">
-        <v>8.5052800000000008</v>
+        <v>5.4637700000000002</v>
       </c>
       <c r="CJ12" s="2">
-        <v>5.9825299999999997</v>
+        <v>5.5136500000000002</v>
       </c>
       <c r="CK12" s="2">
-        <v>5.9964899999999997</v>
+        <v>8.0868500000000001</v>
       </c>
       <c r="CL12" s="2">
-        <v>6.9250800000000003</v>
+        <v>2.0654499999999998</v>
       </c>
       <c r="CM12" s="2">
-        <v>6.49444</v>
+        <v>3.9321600000000001</v>
       </c>
       <c r="CN12" s="2">
-        <v>6.3431699999999998</v>
+        <v>2.5042300000000002</v>
       </c>
       <c r="CO12" s="2">
-        <v>5.9912700000000001</v>
+        <v>5.9447799999999997</v>
       </c>
       <c r="CP12" t="s">
         <v>286</v>
@@ -3581,562 +3584,846 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.2452799999999999</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.73102</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1.64015</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1.77817</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.56850000000000001</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1.76467</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.79384999999999994</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.73258000000000001</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1.22241</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1.2118100000000001</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1.1236699999999999</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1.5549299999999999</v>
-      </c>
-      <c r="O14" s="2">
-        <v>1.11277</v>
-      </c>
-      <c r="P14" s="2">
-        <v>1.0474699999999999</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>0.99802000000000002</v>
-      </c>
-      <c r="R14" s="2">
-        <v>1.3523400000000001</v>
-      </c>
-      <c r="S14" s="2">
-        <v>1.0710900000000001</v>
-      </c>
-      <c r="T14" s="2">
-        <v>0.96518000000000004</v>
-      </c>
-      <c r="U14" s="2">
-        <v>0.94247000000000003</v>
-      </c>
-      <c r="V14" s="2">
-        <v>-1.06471</v>
-      </c>
-      <c r="W14" s="2">
-        <v>1.67276</v>
-      </c>
-      <c r="X14" s="2">
-        <v>-0.73333000000000004</v>
-      </c>
-      <c r="Y14" s="2">
-        <v>0.73509000000000002</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>1.7403200000000001</v>
-      </c>
-      <c r="AA14" s="2">
-        <v>2.56996</v>
-      </c>
-      <c r="AB14" s="2">
-        <v>1.9816100000000001</v>
-      </c>
-      <c r="AC14" s="2">
-        <v>1.64662</v>
-      </c>
-      <c r="AD14" s="2">
-        <v>1.1802600000000001</v>
-      </c>
-      <c r="AE14" s="2">
-        <v>1.7056500000000001</v>
-      </c>
-      <c r="AF14" s="2">
-        <v>1.34832</v>
-      </c>
-      <c r="AG14" s="2">
-        <v>0.95889999999999997</v>
-      </c>
-      <c r="AH14" s="2">
-        <v>1.1231899999999999</v>
-      </c>
-      <c r="AI14" s="2">
-        <v>-0.39773999999999998</v>
-      </c>
-      <c r="AJ14" s="2">
-        <v>0.92922000000000005</v>
-      </c>
-      <c r="AK14" s="2">
-        <v>1.2955399999999999</v>
-      </c>
-      <c r="AL14" s="2">
-        <v>1.6230800000000001</v>
-      </c>
-      <c r="AM14" s="2">
-        <v>0.37853999999999999</v>
-      </c>
-      <c r="AN14" s="2">
-        <v>1.2237499999999999</v>
-      </c>
-      <c r="AO14" s="2">
-        <v>1.11005</v>
-      </c>
-      <c r="AP14" s="2">
-        <v>1.1332500000000001</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>0.82589000000000001</v>
-      </c>
-      <c r="AR14" s="2">
-        <v>1.4808399999999999</v>
-      </c>
-      <c r="AS14" s="2">
-        <v>0.33593000000000001</v>
-      </c>
-      <c r="AT14" s="2">
-        <v>0.68486000000000002</v>
-      </c>
-      <c r="AU14" s="2">
-        <v>2.3804400000000001</v>
-      </c>
-      <c r="AV14" s="2">
-        <v>1.5673699999999999</v>
-      </c>
-      <c r="AW14" s="2">
-        <v>2.2438500000000001</v>
-      </c>
-      <c r="AX14" s="2">
-        <v>0.68201999999999996</v>
-      </c>
-      <c r="AY14" s="2">
-        <v>1.80481</v>
-      </c>
-      <c r="AZ14" s="2">
-        <v>1.67354</v>
-      </c>
-      <c r="BA14" s="2">
-        <v>1.2162599999999999</v>
-      </c>
-      <c r="BB14" s="2">
-        <v>0.36577999999999999</v>
-      </c>
-      <c r="BC14" s="2">
-        <v>2.3016700000000001</v>
-      </c>
-      <c r="BD14" s="2">
-        <v>1.32935</v>
-      </c>
-      <c r="BE14" s="2">
-        <v>1.3167599999999999</v>
-      </c>
-      <c r="BF14" s="2">
-        <v>0.98580000000000001</v>
-      </c>
-      <c r="BG14" s="2">
-        <v>1.6696899999999999</v>
-      </c>
-      <c r="BH14" s="2">
-        <v>0.92159000000000002</v>
-      </c>
-      <c r="BI14" s="2">
-        <v>1.08039</v>
-      </c>
-      <c r="BJ14" s="2">
-        <v>0.75095000000000001</v>
-      </c>
-      <c r="BK14" s="2">
-        <v>1.3260799999999999</v>
-      </c>
-      <c r="BL14" s="2">
-        <v>2.1433499999999999</v>
-      </c>
-      <c r="BM14" s="2">
-        <v>0.89825999999999995</v>
-      </c>
-      <c r="BN14" s="2">
-        <v>2.4283100000000002</v>
-      </c>
-      <c r="BO14" s="2">
-        <v>1.12523</v>
-      </c>
-      <c r="BP14" s="2">
-        <v>0.99180999999999997</v>
-      </c>
-      <c r="BQ14" s="2">
-        <v>2.07457</v>
-      </c>
-      <c r="BR14" s="2">
-        <v>1.1291800000000001</v>
-      </c>
-      <c r="BS14" s="2">
-        <v>0.65888999999999998</v>
-      </c>
-      <c r="BT14" s="2">
-        <v>0.68162999999999996</v>
-      </c>
-      <c r="BU14" s="2">
-        <v>1.9415</v>
-      </c>
-      <c r="BV14" s="2">
-        <v>1.8282700000000001</v>
-      </c>
-      <c r="BW14" s="2">
-        <v>0.92803000000000002</v>
-      </c>
-      <c r="BX14" s="2">
-        <v>1.3465199999999999</v>
-      </c>
-      <c r="BY14" s="2">
-        <v>1.1127899999999999</v>
-      </c>
-      <c r="BZ14" s="2">
-        <v>0.83070999999999995</v>
-      </c>
-      <c r="CA14" s="2">
-        <v>0.71570999999999996</v>
-      </c>
-      <c r="CB14" s="2">
-        <v>1.8677600000000001</v>
-      </c>
-      <c r="CC14" s="2">
-        <v>1.6599900000000001</v>
-      </c>
-      <c r="CD14" s="2">
-        <v>0.65619000000000005</v>
-      </c>
-      <c r="CE14" s="2">
-        <v>1.6655899999999999</v>
-      </c>
-      <c r="CF14" s="2">
-        <v>1.9583999999999999</v>
-      </c>
-      <c r="CG14" s="2">
-        <v>1.26908</v>
-      </c>
-      <c r="CH14" s="2">
-        <v>1.97288</v>
-      </c>
-      <c r="CI14" s="2">
-        <v>1.7742500000000001</v>
-      </c>
-      <c r="CJ14" s="2">
-        <v>0.85163</v>
-      </c>
-      <c r="CK14" s="2">
-        <v>1.5718799999999999</v>
-      </c>
-      <c r="CL14" s="2">
-        <v>1.7406600000000001</v>
-      </c>
-      <c r="CM14" s="2">
-        <v>1.2820499999999999</v>
-      </c>
-      <c r="CN14" s="2">
-        <v>1.3283700000000001</v>
-      </c>
-      <c r="CO14" s="2">
-        <v>1.49448</v>
+    <row r="13" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10.158770000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.4727499999999996</v>
+      </c>
+      <c r="E13" s="2">
+        <v>7.4537000000000004</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.3738299999999999</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.9239600000000001</v>
+      </c>
+      <c r="H13" s="2">
+        <v>7.4272499999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.1239100000000004</v>
+      </c>
+      <c r="J13" s="2">
+        <v>8.5286899999999992</v>
+      </c>
+      <c r="K13" s="2">
+        <v>6.2963199999999997</v>
+      </c>
+      <c r="L13" s="2">
+        <v>8.7127300000000005</v>
+      </c>
+      <c r="M13" s="2">
+        <v>10.038259999999999</v>
+      </c>
+      <c r="N13" s="2">
+        <v>8.3004899999999999</v>
+      </c>
+      <c r="O13" s="2">
+        <v>9.3532299999999999</v>
+      </c>
+      <c r="P13" s="2">
+        <v>6.5704200000000004</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>9.1646699999999992</v>
+      </c>
+      <c r="R13" s="2">
+        <v>6.2262199999999996</v>
+      </c>
+      <c r="S13" s="2">
+        <v>7.17774</v>
+      </c>
+      <c r="T13" s="2">
+        <v>6.3941800000000004</v>
+      </c>
+      <c r="U13" s="2">
+        <v>6.9149000000000003</v>
+      </c>
+      <c r="V13" s="2">
+        <v>5.8858800000000002</v>
+      </c>
+      <c r="W13" s="2">
+        <v>7.5102500000000001</v>
+      </c>
+      <c r="X13" s="2">
+        <v>3.80145</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>4.8563599999999996</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>5.9795199999999999</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>9.2229299999999999</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>9.2211099999999995</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>8.3966899999999995</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>7.4177499999999998</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>8.1916600000000006</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>6.0623300000000002</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>9.1206700000000005</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>6.2064899999999996</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>3.12277</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>7.13347</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>5.5058299999999996</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>6.57064</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>5.57456</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>5.6974900000000002</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>10.532019999999999</v>
+      </c>
+      <c r="AP13" s="2">
+        <v>4.6502100000000004</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>5.2417499999999997</v>
+      </c>
+      <c r="AR13" s="2">
+        <v>7.7904299999999997</v>
+      </c>
+      <c r="AS13" s="2">
+        <v>4.2834199999999996</v>
+      </c>
+      <c r="AT13" s="2">
+        <v>6.7729100000000004</v>
+      </c>
+      <c r="AU13" s="2">
+        <v>8.7543600000000001</v>
+      </c>
+      <c r="AV13" s="2">
+        <v>6.0541999999999998</v>
+      </c>
+      <c r="AW13" s="2">
+        <v>8.0451899999999998</v>
+      </c>
+      <c r="AX13" s="2">
+        <v>5.39635</v>
+      </c>
+      <c r="AY13" s="2">
+        <v>10.5456</v>
+      </c>
+      <c r="AZ13" s="2">
+        <v>7.3565100000000001</v>
+      </c>
+      <c r="BA13" s="2">
+        <v>6.7207600000000003</v>
+      </c>
+      <c r="BB13" s="2">
+        <v>3.4305500000000002</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>9.7064699999999995</v>
+      </c>
+      <c r="BD13" s="2">
+        <v>6.1847399999999997</v>
+      </c>
+      <c r="BE13" s="2">
+        <v>5.1341099999999997</v>
+      </c>
+      <c r="BF13" s="2">
+        <v>5.9257099999999996</v>
+      </c>
+      <c r="BG13" s="2">
+        <v>6.2577100000000003</v>
+      </c>
+      <c r="BH13" s="2">
+        <v>7.2429300000000003</v>
+      </c>
+      <c r="BI13" s="2">
+        <v>7.8703099999999999</v>
+      </c>
+      <c r="BJ13" s="2">
+        <v>5.3787099999999999</v>
+      </c>
+      <c r="BK13" s="2">
+        <v>8.0756599999999992</v>
+      </c>
+      <c r="BL13" s="2">
+        <v>8.9649199999999993</v>
+      </c>
+      <c r="BM13" s="2">
+        <v>7.9430699999999996</v>
+      </c>
+      <c r="BN13" s="2">
+        <v>8.7584700000000009</v>
+      </c>
+      <c r="BO13" s="2">
+        <v>6.3030999999999997</v>
+      </c>
+      <c r="BP13" s="2">
+        <v>6.1244800000000001</v>
+      </c>
+      <c r="BQ13" s="2">
+        <v>6.0146199999999999</v>
+      </c>
+      <c r="BR13" s="2">
+        <v>6.3564400000000001</v>
+      </c>
+      <c r="BS13" s="2">
+        <v>6.6078400000000004</v>
+      </c>
+      <c r="BT13" s="2">
+        <v>5.93649</v>
+      </c>
+      <c r="BU13" s="2">
+        <v>8.8595600000000001</v>
+      </c>
+      <c r="BV13" s="2">
+        <v>6.8673400000000004</v>
+      </c>
+      <c r="BW13" s="2">
+        <v>6.3774600000000001</v>
+      </c>
+      <c r="BX13" s="2">
+        <v>6.64602</v>
+      </c>
+      <c r="BY13" s="2">
+        <v>7.3281200000000002</v>
+      </c>
+      <c r="BZ13" s="2">
+        <v>7.0018399999999996</v>
+      </c>
+      <c r="CA13" s="2">
+        <v>6.7076700000000002</v>
+      </c>
+      <c r="CB13" s="2">
+        <v>8.1388599999999993</v>
+      </c>
+      <c r="CC13" s="2">
+        <v>4.6814900000000002</v>
+      </c>
+      <c r="CD13" s="2">
+        <v>6.4156700000000004</v>
+      </c>
+      <c r="CE13" s="2">
+        <v>8.4468200000000007</v>
+      </c>
+      <c r="CF13" s="2">
+        <v>7.7824900000000001</v>
+      </c>
+      <c r="CG13" s="2">
+        <v>6.5670400000000004</v>
+      </c>
+      <c r="CH13" s="2">
+        <v>9.1699900000000003</v>
+      </c>
+      <c r="CI13" s="2">
+        <v>8.5052800000000008</v>
+      </c>
+      <c r="CJ13" s="2">
+        <v>5.9825299999999997</v>
+      </c>
+      <c r="CK13" s="2">
+        <v>5.9964899999999997</v>
+      </c>
+      <c r="CL13" s="2">
+        <v>6.9250800000000003</v>
+      </c>
+      <c r="CM13" s="2">
+        <v>6.49444</v>
+      </c>
+      <c r="CN13" s="2">
+        <v>6.3431699999999998</v>
+      </c>
+      <c r="CO13" s="2">
+        <v>5.9912700000000001</v>
+      </c>
+      <c r="CP13" t="s">
+        <v>286</v>
+      </c>
+      <c r="CQ13" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:95" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.2452799999999999</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.73102</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.64015</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.77817</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.56850000000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.76467</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.79384999999999994</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.73258000000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.22241</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.2118100000000001</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.1236699999999999</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1.5549299999999999</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.11277</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1.0474699999999999</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0.99802000000000002</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1.3523400000000001</v>
+      </c>
+      <c r="S15" s="2">
+        <v>1.0710900000000001</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0.96518000000000004</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0.94247000000000003</v>
+      </c>
+      <c r="V15" s="2">
+        <v>-1.06471</v>
+      </c>
+      <c r="W15" s="2">
+        <v>1.67276</v>
+      </c>
+      <c r="X15" s="2">
+        <v>-0.73333000000000004</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0.73509000000000002</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1.7403200000000001</v>
+      </c>
+      <c r="AA15" s="2">
+        <v>2.56996</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>1.9816100000000001</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>1.64662</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>1.1802600000000001</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>1.7056500000000001</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>1.34832</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>0.95889999999999997</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>1.1231899999999999</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>-0.39773999999999998</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>0.92922000000000005</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>1.2955399999999999</v>
+      </c>
+      <c r="AL15" s="2">
+        <v>1.6230800000000001</v>
+      </c>
+      <c r="AM15" s="2">
+        <v>0.37853999999999999</v>
+      </c>
+      <c r="AN15" s="2">
+        <v>1.2237499999999999</v>
+      </c>
+      <c r="AO15" s="2">
+        <v>1.11005</v>
+      </c>
+      <c r="AP15" s="2">
+        <v>1.1332500000000001</v>
+      </c>
+      <c r="AQ15" s="2">
+        <v>0.82589000000000001</v>
+      </c>
+      <c r="AR15" s="2">
+        <v>1.4808399999999999</v>
+      </c>
+      <c r="AS15" s="2">
+        <v>0.33593000000000001</v>
+      </c>
+      <c r="AT15" s="2">
+        <v>0.68486000000000002</v>
+      </c>
+      <c r="AU15" s="2">
+        <v>2.3804400000000001</v>
+      </c>
+      <c r="AV15" s="2">
+        <v>1.5673699999999999</v>
+      </c>
+      <c r="AW15" s="2">
+        <v>2.2438500000000001</v>
+      </c>
+      <c r="AX15" s="2">
+        <v>0.68201999999999996</v>
+      </c>
+      <c r="AY15" s="2">
+        <v>1.80481</v>
+      </c>
+      <c r="AZ15" s="2">
+        <v>1.67354</v>
+      </c>
+      <c r="BA15" s="2">
+        <v>1.2162599999999999</v>
+      </c>
+      <c r="BB15" s="2">
+        <v>0.36577999999999999</v>
+      </c>
+      <c r="BC15" s="2">
+        <v>2.3016700000000001</v>
+      </c>
+      <c r="BD15" s="2">
+        <v>1.32935</v>
+      </c>
+      <c r="BE15" s="2">
+        <v>1.3167599999999999</v>
+      </c>
+      <c r="BF15" s="2">
+        <v>0.98580000000000001</v>
+      </c>
+      <c r="BG15" s="2">
+        <v>1.6696899999999999</v>
+      </c>
+      <c r="BH15" s="2">
+        <v>0.92159000000000002</v>
+      </c>
+      <c r="BI15" s="2">
+        <v>1.08039</v>
+      </c>
+      <c r="BJ15" s="2">
+        <v>0.75095000000000001</v>
+      </c>
+      <c r="BK15" s="2">
+        <v>1.3260799999999999</v>
+      </c>
+      <c r="BL15" s="2">
+        <v>2.1433499999999999</v>
+      </c>
+      <c r="BM15" s="2">
+        <v>0.89825999999999995</v>
+      </c>
+      <c r="BN15" s="2">
+        <v>2.4283100000000002</v>
+      </c>
+      <c r="BO15" s="2">
+        <v>1.12523</v>
+      </c>
+      <c r="BP15" s="2">
+        <v>0.99180999999999997</v>
+      </c>
+      <c r="BQ15" s="2">
+        <v>2.07457</v>
+      </c>
+      <c r="BR15" s="2">
+        <v>1.1291800000000001</v>
+      </c>
+      <c r="BS15" s="2">
+        <v>0.65888999999999998</v>
+      </c>
+      <c r="BT15" s="2">
+        <v>0.68162999999999996</v>
+      </c>
+      <c r="BU15" s="2">
+        <v>1.9415</v>
+      </c>
+      <c r="BV15" s="2">
+        <v>1.8282700000000001</v>
+      </c>
+      <c r="BW15" s="2">
+        <v>0.92803000000000002</v>
+      </c>
+      <c r="BX15" s="2">
+        <v>1.3465199999999999</v>
+      </c>
+      <c r="BY15" s="2">
+        <v>1.1127899999999999</v>
+      </c>
+      <c r="BZ15" s="2">
+        <v>0.83070999999999995</v>
+      </c>
+      <c r="CA15" s="2">
+        <v>0.71570999999999996</v>
+      </c>
+      <c r="CB15" s="2">
+        <v>1.8677600000000001</v>
+      </c>
+      <c r="CC15" s="2">
+        <v>1.6599900000000001</v>
+      </c>
+      <c r="CD15" s="2">
+        <v>0.65619000000000005</v>
+      </c>
+      <c r="CE15" s="2">
+        <v>1.6655899999999999</v>
+      </c>
+      <c r="CF15" s="2">
+        <v>1.9583999999999999</v>
+      </c>
+      <c r="CG15" s="2">
+        <v>1.26908</v>
+      </c>
+      <c r="CH15" s="2">
+        <v>1.97288</v>
+      </c>
+      <c r="CI15" s="2">
+        <v>1.7742500000000001</v>
+      </c>
+      <c r="CJ15" s="2">
+        <v>0.85163</v>
+      </c>
+      <c r="CK15" s="2">
+        <v>1.5718799999999999</v>
+      </c>
+      <c r="CL15" s="2">
+        <v>1.7406600000000001</v>
+      </c>
+      <c r="CM15" s="2">
+        <v>1.2820499999999999</v>
+      </c>
+      <c r="CN15" s="2">
+        <v>1.3283700000000001</v>
+      </c>
+      <c r="CO15" s="2">
+        <v>1.49448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:95" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>290</v>
       </c>
-      <c r="B15" s="6">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E16" s="6">
         <v>0.25</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F16" s="6">
         <v>0.75</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6">
-        <v>0</v>
-      </c>
-      <c r="K15" s="6">
-        <v>0</v>
-      </c>
-      <c r="L15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
         <v>0.5</v>
       </c>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="P15" s="6">
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
         <v>0.75</v>
       </c>
-      <c r="Q15" s="6">
-        <v>0</v>
-      </c>
-      <c r="R15" s="6">
-        <v>0</v>
-      </c>
-      <c r="S15" s="6">
-        <v>0</v>
-      </c>
-      <c r="T15" s="6">
+      <c r="Q16" s="6">
+        <v>0</v>
+      </c>
+      <c r="R16" s="6">
+        <v>0</v>
+      </c>
+      <c r="S16" s="6">
+        <v>0</v>
+      </c>
+      <c r="T16" s="6">
         <v>0.75</v>
       </c>
-      <c r="U15" s="6">
-        <v>0</v>
-      </c>
-      <c r="V15" s="6">
-        <v>0</v>
-      </c>
-      <c r="W15" s="6">
+      <c r="U16" s="6">
+        <v>0</v>
+      </c>
+      <c r="V16" s="6">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6">
         <v>0.75</v>
       </c>
-      <c r="X15" s="6">
+      <c r="X16" s="6">
         <v>0.75</v>
       </c>
-      <c r="Y15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="6">
+      <c r="Y16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AA15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="6">
+      <c r="AA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AC15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="6">
+      <c r="AC16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="6">
         <v>0.25</v>
       </c>
-      <c r="AH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="6">
+      <c r="AH16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="6">
         <v>0.25</v>
       </c>
-      <c r="AM15" s="6">
+      <c r="AM16" s="6">
         <v>0.5</v>
       </c>
-      <c r="AN15" s="6">
+      <c r="AN16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AO15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AP15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AQ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AS15" s="6">
+      <c r="AO16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="6">
         <v>0.5</v>
       </c>
-      <c r="AT15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AU15" s="6">
+      <c r="AT16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="6">
         <v>0.75</v>
       </c>
-      <c r="AV15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AW15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AX15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AY15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AZ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BA15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BB15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BC15" s="6">
+      <c r="AV16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AX16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BD15" s="6">
+      <c r="BD16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BE15" s="6">
+      <c r="BE16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BF15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BG15" s="6">
+      <c r="BF16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BG16" s="6">
         <v>0.25</v>
       </c>
-      <c r="BH15" s="6">
+      <c r="BH16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BI15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BJ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BL15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BM15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BN15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BO15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BP15" s="6">
+      <c r="BI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BK16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BM16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BN16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BO16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BP16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BQ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BR15" s="6">
+      <c r="BQ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BR16" s="6">
         <v>0.5</v>
       </c>
-      <c r="BS15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BT15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BU15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BV15" s="6">
+      <c r="BS16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BT16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BU16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BV16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BW15" s="6">
+      <c r="BW16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BX15" s="6">
-        <v>0</v>
-      </c>
-      <c r="BY15" s="6">
+      <c r="BX16" s="6">
+        <v>0</v>
+      </c>
+      <c r="BY16" s="6">
         <v>0.75</v>
       </c>
-      <c r="BZ15" s="6">
+      <c r="BZ16" s="6">
         <v>0.75</v>
       </c>
-      <c r="CA15" s="6">
+      <c r="CA16" s="6">
         <v>0.75</v>
       </c>
-      <c r="CB15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CC15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CD15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CE15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CF15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CG15" s="6">
+      <c r="CB16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CC16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CD16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CE16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CF16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CG16" s="6">
         <v>0.25</v>
       </c>
-      <c r="CH15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CI15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CJ15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CL15" s="6">
+      <c r="CH16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CI16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CJ16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CK16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CL16" s="6">
         <v>0.5</v>
       </c>
-      <c r="CM15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CN15" s="6">
-        <v>0</v>
-      </c>
-      <c r="CO15" s="6">
+      <c r="CM16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CN16" s="6">
+        <v>0</v>
+      </c>
+      <c r="CO16" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>